<commit_message>
Added all CSVs with Indicator Tags
</commit_message>
<xml_diff>
--- a/City Projects /round-1/20-Bhopal_projects.xlsx
+++ b/City Projects /round-1/20-Bhopal_projects.xlsx
@@ -1,10 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10910"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/cxphan/Downloads/Remote Repos/India - Smart Cities Feature Extraction/City Projects /round-1/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5EB304FE-3A95-F446-B97B-E9EB5F14AE74}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="15" windowWidth="18960" windowHeight="11325"/>
+    <workbookView xWindow="120" yWindow="460" windowWidth="18960" windowHeight="11320" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Table 1" sheetId="1" r:id="rId1"/>
@@ -14,86 +20,86 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="22">
   <si>
     <r>
       <rPr>
         <b/>
-        <sz val="9.0"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">List of Projects as per Smart City Proposal : Bhopal</t>
+        <sz val="9"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>List of Projects as per Smart City Proposal : Bhopal</t>
     </r>
   </si>
   <si>
     <r>
       <rPr>
         <b/>
-        <sz val="9.0"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">Sl. No.</t>
+        <sz val="9"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>Sl. No.</t>
     </r>
   </si>
   <si>
     <r>
       <rPr>
         <b/>
-        <sz val="9.0"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">Projects in SCP</t>
+        <sz val="9"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>Projects in SCP</t>
     </r>
   </si>
   <si>
     <r>
       <rPr>
         <b/>
-        <sz val="9.0"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">Cost (Rs. in Crore)</t>
+        <sz val="9"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>Cost (Rs. in Crore)</t>
     </r>
   </si>
   <si>
     <r>
       <rPr>
         <b/>
-        <sz val="9.0"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">Area Based Development (ABD)</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="9.0"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">Electricity provision and Energy Efficiency  (Assured electricity supply with at least 10% of the energy requirement coming from solar, Smart metering, Energy efficient street lighting, Energy efficiency for 80% of buildings)</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="9.0"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">Sanitation  (Sanitation including SWM)</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="9.0"/>
+        <sz val="9"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>Area Based Development (ABD)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>Electricity provision and Energy Efficiency  (Assured electricity supply with at least 10% of the energy requirement coming from solar, Smart metering, Energy efficient street lighting, Energy efficiency for 80% of buildings)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>Sanitation  (Sanitation including SWM)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="9"/>
         <rFont val="Calibri"/>
         <family val="2"/>
       </rPr>
@@ -102,17 +108,17 @@
     </r>
     <r>
       <rPr>
-        <sz val="9.0"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">(Robust IT connectivity and digitalization, Intelligent traffic management, Smart parking, Safety of citizens, Additional Smart Applications)</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="9.0"/>
+        <sz val="9"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>(Robust IT connectivity and digitalization, Intelligent traffic management, Smart parking, Safety of citizens, Additional Smart Applications)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="9"/>
         <rFont val="Calibri"/>
         <family val="2"/>
       </rPr>
@@ -121,17 +127,17 @@
     </r>
     <r>
       <rPr>
-        <sz val="9.0"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">(Adequate water supply including waste water recycling and storm water reuse, Rain water harvesting)</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="9.0"/>
+        <sz val="9"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>(Adequate water supply including waste water recycling and storm water reuse, Rain water harvesting)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="9"/>
         <rFont val="Calibri"/>
         <family val="2"/>
       </rPr>
@@ -140,17 +146,17 @@
     </r>
     <r>
       <rPr>
-        <sz val="9.0"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">(Pedestrian friendly pathways, Encouragement to non-motorised transport, Non- vehicle streets/zones)</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="9.0"/>
+        <sz val="9"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>(Pedestrian friendly pathways, Encouragement to non-motorised transport, Non- vehicle streets/zones)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="9"/>
         <rFont val="Calibri"/>
         <family val="2"/>
       </rPr>
@@ -159,17 +165,17 @@
     </r>
     <r>
       <rPr>
-        <sz val="9.0"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">(nnovative use of open spaces, Visible improvement  in the Area)</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="9.0"/>
+        <sz val="9"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>(nnovative use of open spaces, Visible improvement  in the Area)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="9"/>
         <rFont val="Calibri"/>
         <family val="2"/>
       </rPr>
@@ -178,28 +184,28 @@
     </r>
     <r>
       <rPr>
-        <sz val="9.0"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">15% affordable housing)</t>
+        <sz val="9"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>15% affordable housing)</t>
     </r>
   </si>
   <si>
     <r>
       <rPr>
         <b/>
-        <sz val="9.0"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">Pan City</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="9.0"/>
+        <sz val="9"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>Pan City</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="9"/>
         <rFont val="Calibri"/>
         <family val="2"/>
       </rPr>
@@ -208,17 +214,17 @@
     </r>
     <r>
       <rPr>
-        <sz val="9.0"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">(Ease of doing Business applications, Citizen engagement and grievance module, City level application and smart dashboard, Data Analytics and MIS, City Level GIS, Mobile service delivery, Waste to Energy conversion, GPS based garbage vehicle tracking, Asset and operation management  system, RFID tagging of garbage bins, Waste network simulation, GIS based grievance redressal, Geo- fencing of assets)</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="9.0"/>
+        <sz val="9"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>(Ease of doing Business applications, Citizen engagement and grievance module, City level application and smart dashboard, Data Analytics and MIS, City Level GIS, Mobile service delivery, Waste to Energy conversion, GPS based garbage vehicle tracking, Asset and operation management  system, RFID tagging of garbage bins, Waste network simulation, GIS based grievance redressal, Geo- fencing of assets)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="9"/>
         <rFont val="Calibri"/>
         <family val="2"/>
       </rPr>
@@ -227,17 +233,17 @@
     </r>
     <r>
       <rPr>
-        <sz val="9.0"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">(Intelligent street light with scheduling,  Surveillance and SOS, Environment and water level sensors, Wi-Fi, Intelligent shopping apps, Smart phone detection, Interactive digital signage</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="9.0"/>
+        <sz val="9"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>(Intelligent street light with scheduling,  Surveillance and SOS, Environment and water level sensors, Wi-Fi, Intelligent shopping apps, Smart phone detection, Interactive digital signage</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="9"/>
         <rFont val="Calibri"/>
         <family val="2"/>
       </rPr>
@@ -246,44 +252,37 @@
     </r>
     <r>
       <rPr>
-        <sz val="9.0"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">(Landscaping, Flyovers to approach site, Development of public utilities)</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b/>
-        <i/>
-        <sz val="6.5"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">Note-  </t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="6.5"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">This only indicates cost of individual projects given in the SCP. The total value of SCP may additionally include other costs such as DPR preparation, PMC, O&amp;M etc.</t>
-    </r>
+        <sz val="9"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>(Landscaping, Flyovers to approach site, Development of public utilities)</t>
+    </r>
+  </si>
+  <si>
+    <t>City-Projects</t>
+  </si>
+  <si>
+    <t>Size</t>
+  </si>
+  <si>
+    <t>Indicator</t>
+  </si>
+  <si>
+    <t>ABD</t>
+  </si>
+  <si>
+    <t>N/A</t>
+  </si>
+  <si>
+    <t>Pan City</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="2">
-    <numFmt numFmtId="164" formatCode="0"/>
-    <numFmt numFmtId="165" formatCode="0.00"/>
-  </numFmts>
-  <fonts count="4">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -305,6 +304,17 @@
       <sz val="9"/>
       <name val="Calibri"/>
     </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -319,7 +329,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="6">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -377,67 +387,52 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color rgb="FF000000"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
-    <xf numFmtId="0" fillId="0" borderId="0" fontId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+  <cellXfs count="14">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fillId="0" borderId="1" fontId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" indent="19" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fillId="2" borderId="2" fontId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fillId="2" borderId="2" fontId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" indent="3" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fillId="0" borderId="2" fontId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="bottom" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fillId="0" borderId="2" fontId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1" indent="3"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="2" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fillId="0" borderId="3" fontId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="2" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fillId="0" borderId="4" fontId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="1" fontId="2" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="2" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="2" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1" indent="19"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fillId="0" borderId="2" fontId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fillId="0" borderId="2" fontId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="165" fillId="0" borderId="2" fontId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fillId="0" borderId="2" fontId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fillId="0" borderId="2" fontId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="165" fillId="0" borderId="2" fontId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="164" fillId="0" borderId="2" fontId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fillId="0" borderId="5" fontId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -445,6 +440,14 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -491,7 +494,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -523,9 +526,27 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -557,6 +578,24 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -732,173 +771,236 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C15"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:F14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B12" sqref="B12"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" customWidth="1" width="12.666667"/>
-    <col min="2" max="2" customWidth="1" width="71.111111"/>
-    <col min="3" max="3" customWidth="1" width="26.666667"/>
+    <col min="1" max="1" width="12.59765625" customWidth="1"/>
+    <col min="2" max="2" width="71.19921875" customWidth="1"/>
+    <col min="3" max="3" width="26.59765625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="16.50" customHeight="1">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A1" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1"/>
-      <c r="C1" s="1"/>
-    </row>
-    <row r="2" spans="1:3" ht="13.50" customHeight="1">
-      <c r="A2" s="2" t="s">
+      <c r="B1" s="11"/>
+      <c r="C1" s="11"/>
+    </row>
+    <row r="2" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="B2" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="C2" s="2" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" ht="13.50" customHeight="1">
-      <c r="A3" s="4"/>
-      <c r="B3" s="6" t="s">
+      <c r="D2" t="s">
+        <v>16</v>
+      </c>
+      <c r="E2" t="s">
+        <v>17</v>
+      </c>
+      <c r="F2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A3" s="3"/>
+      <c r="B3" s="12" t="s">
         <v>4</v>
       </c>
-      <c r="C3" s="7"/>
-    </row>
-    <row r="4" spans="1:3" ht="46.25" customHeight="1">
-      <c r="A4" s="8">
+      <c r="C3" s="13"/>
+    </row>
+    <row r="4" spans="1:6" ht="46.25" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A4" s="4">
         <v>1</v>
       </c>
-      <c r="B4" s="9" t="s">
+      <c r="B4" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="C4" s="10">
-        <v>120.00</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" ht="13.50" customHeight="1">
-      <c r="A5" s="8">
+      <c r="C4" s="6">
+        <v>120</v>
+      </c>
+      <c r="D4" t="s">
+        <v>20</v>
+      </c>
+      <c r="E4" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A5" s="4">
         <v>2</v>
       </c>
-      <c r="B5" s="9" t="s">
+      <c r="B5" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="C5" s="10">
-        <v>50.50</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" ht="46.25" customHeight="1">
-      <c r="A6" s="8">
+      <c r="C5" s="6">
+        <v>50.5</v>
+      </c>
+      <c r="D5" t="s">
+        <v>20</v>
+      </c>
+      <c r="E5" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" ht="46.25" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A6" s="4">
         <v>3</v>
       </c>
-      <c r="B6" s="11" t="s">
+      <c r="B6" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="C6" s="10">
-        <v>150.00</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" ht="34.75" customHeight="1">
-      <c r="A7" s="12">
+      <c r="C6" s="6">
+        <v>150</v>
+      </c>
+      <c r="D6" t="s">
+        <v>20</v>
+      </c>
+      <c r="E6" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" ht="34.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A7" s="8">
         <v>4</v>
       </c>
-      <c r="B7" s="11" t="s">
+      <c r="B7" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="C7" s="13">
-        <v>86.00</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" ht="34.75" customHeight="1">
-      <c r="A8" s="12">
+      <c r="C7" s="9">
+        <v>86</v>
+      </c>
+      <c r="D7" t="s">
+        <v>20</v>
+      </c>
+      <c r="E7" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" ht="34.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A8" s="8">
         <v>5</v>
       </c>
-      <c r="B8" s="11" t="s">
+      <c r="B8" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="C8" s="13">
-        <v>95.00</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" ht="27.00" customHeight="1">
-      <c r="A9" s="8">
+      <c r="C8" s="9">
+        <v>95</v>
+      </c>
+      <c r="D8" t="s">
+        <v>20</v>
+      </c>
+      <c r="E8" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" ht="27" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A9" s="4">
         <v>6</v>
       </c>
-      <c r="B9" s="11" t="s">
+      <c r="B9" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="C9" s="10">
-        <v>20.00</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" ht="27.00" customHeight="1">
-      <c r="A10" s="8">
+      <c r="C9" s="6">
+        <v>20</v>
+      </c>
+      <c r="D9" t="s">
+        <v>20</v>
+      </c>
+      <c r="E9" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" ht="27" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A10" s="4">
         <v>7</v>
       </c>
-      <c r="B10" s="11" t="s">
+      <c r="B10" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="C10" s="10">
-        <v>922.00</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" ht="13.50" customHeight="1">
-      <c r="A11" s="4"/>
-      <c r="B11" s="6" t="s">
+      <c r="C10" s="6">
+        <v>922</v>
+      </c>
+      <c r="D10" t="s">
+        <v>20</v>
+      </c>
+      <c r="E10" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A11" s="3"/>
+      <c r="B11" s="12" t="s">
         <v>12</v>
       </c>
-      <c r="C11" s="7"/>
-    </row>
-    <row r="12" spans="1:3" ht="105.75" customHeight="1">
-      <c r="A12" s="12">
+      <c r="C11" s="13"/>
+    </row>
+    <row r="12" spans="1:6" ht="105.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A12" s="8">
         <v>8</v>
       </c>
-      <c r="B12" s="11" t="s">
+      <c r="B12" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="C12" s="13">
-        <v>200.00</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" ht="59.00" customHeight="1">
-      <c r="A13" s="12">
+      <c r="C12" s="9">
+        <v>200</v>
+      </c>
+      <c r="D12" t="s">
+        <v>20</v>
+      </c>
+      <c r="E12" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" ht="59" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A13" s="8">
         <v>9</v>
       </c>
-      <c r="B13" s="11" t="s">
+      <c r="B13" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="C13" s="13">
+      <c r="C13" s="9">
         <v>448.21</v>
       </c>
-    </row>
-    <row r="14" spans="1:3" ht="34.75" customHeight="1">
-      <c r="A14" s="12">
+      <c r="D13" t="s">
+        <v>20</v>
+      </c>
+      <c r="E13" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" ht="34.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A14" s="8">
         <v>10</v>
       </c>
-      <c r="B14" s="11" t="s">
+      <c r="B14" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="C14" s="14">
+      <c r="C14" s="10">
         <v>627</v>
       </c>
-    </row>
-    <row r="15" spans="1:3" ht="21.00" customHeight="1">
-      <c r="A15" s="15" t="s">
-        <v>16</v>
-      </c>
-      <c r="B15" s="15"/>
-      <c r="C15" s="15"/>
+      <c r="D14" t="s">
+        <v>20</v>
+      </c>
+      <c r="E14" t="s">
+        <v>21</v>
+      </c>
     </row>
   </sheetData>
-  <mergeCells count="4">
+  <mergeCells count="3">
     <mergeCell ref="A1:C1"/>
     <mergeCell ref="B3:C3"/>
     <mergeCell ref="B11:C11"/>
-    <mergeCell ref="A15:C15"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>